<commit_message>
Added plate ID and well position
</commit_message>
<xml_diff>
--- a/kinase-expression-constructs/addgene_hip_sgc/selected-kinases.xlsx
+++ b/kinase-expression-constructs/addgene_hip_sgc/selected-kinases.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="507">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="539">
   <si>
     <t>A02</t>
   </si>
@@ -29,12 +29,18 @@
     <t>A09</t>
   </si>
   <si>
+    <t>A1</t>
+  </si>
+  <si>
     <t>A10</t>
   </si>
   <si>
     <t>A12</t>
   </si>
   <si>
+    <t>A3</t>
+  </si>
+  <si>
     <t>AACTTCCGCGTCGGCAAGAAGATCGGCTGCGGCAACTTCGGGGAGCTCCGCCTAGGAAAGAATCTCTATACAAATGAATACGTGGCTATCAAATTGGAGCCGATCAAGTCCCGGGCCCCGCAGCTGCACCTGGAGTACCGGTTCTACAAGCAGCTCAGCGCCACAGAGGGCGTCCCTCAGGTCTACTACTTCGGTCCGTGCGGGAATTACAACGCCATGGTGCTGGAGCTGCTGGGGCCCAGCCTGGAGGACCTGTTCGACCTGTGCGACCGGACCTTCACGCTCAAGACGGTGCTGATGATCGCCATCCAGCTGATCACGCGCATGGAGTATGTGCACACCAAGAGCCTAATCTACCGGGACGTGAAGCCCGAGAACTTCCTGGTGGGCCGCCCGGGGACCAAGCGGCAGCATGCCATCCACATCATCGACTTCGGGCTGGCCAAGGAGTACATCGACCCCGAGACCAAGAAGCACATCCCGTACCGCGAGCACAAGAGCCTGACGGGCACGGCGCGCTACATGAGCATCAACACGCACCTGGGCAAGGAGCAGAGCCGCCGCGACGACCTGGAGGCGCTGGGCCACATGTTCATGTACTTCCTGCGCGGCAGCCTCCCCTGGCAGGGGCTCAAGGCCGACACGCTCAAGGAGCGGTACCAGAAGATCGGGGACACCAAACGCGCCACGCCCATCGAGGTGCTCTGCGAGAACTTCCCAGAGGAGATGGCCACGTACCTGCGCTATGTGCGGCGCCTGGACTTCTTCGAGAAGCCCGACTATGACTACCTGCGGAAGCTCTTCACCGACCTCTTCGACCGCAGTGGCTTCGTGTTCGACTATGAGTACGACTGGGCCGGGAAGCCCCTGCCGACCCCCATCGGCACCGTCCACACCGACCTGCCCTCCCAGCCTCAGCTCCGGGAC</t>
   </si>
   <si>
@@ -506,6 +512,15 @@
     <t>B11</t>
   </si>
   <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>B6</t>
+  </si>
+  <si>
     <t>BMPR2A-c019</t>
   </si>
   <si>
@@ -533,9 +548,21 @@
     <t>C07</t>
   </si>
   <si>
+    <t>C1</t>
+  </si>
+  <si>
     <t>C12</t>
   </si>
   <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
     <t>CACATTGGAAACTACCGGCTCCTCAAGACCATTGGCAAGGGTAATTTTGCCAAGGTGAAGTTGGCCCGACACATCCTGACTGGGAAAGAGGTAGCTGTGAAGATCATTGACAAGACTCAACTGAACTCCTCCAGCCTCCAGAAACTATTCCGCGAAGTAAGAATAATGAAGGTTTTGAATCATCCCAACATAGTTAAATTATTTGAAGTGATTGAGACTGAGAAAACGCTCTACCTTGTCATGGAGTACGCTAGTGGCGGAGAGGTATTTGATTACCTAGTGGCTCATGGCAGGATGAAAGAAAAAGAGGCTCGAGCCAAATTCCGCCAGATAGTGTCTGCTGTGCAGTACTGTCACCAGAAGTTTATTGTCCATAGAGACTTAAAGGCAGAAAACCTGCTCTTGGATGCTGATATGAACATCAAGATTGCAGACTTTGGCTTCAGCAATGAATTCACCTTTGGGAACAAGCTGGACACCTTCTGTGGCAGTCCCCCTTATGCTGCCCCAGAACTCTTCCAGGGCAAAAAATATGATGGACCCGAGGTGGATGTGTGGAGCCTAGGAGTTATCCTCTATACACTGGTCAGCGGATCCCTGCCTTTTGATGGACAGAACCTCAAGGAGCTGCGGGAACGGGTACTGAGGGGAAAATACCGTATTCCATTCTACATGTCCACGGACTGTGAAAACCTGCTTAAGAAATTTCTCATTCTTAATCCCAGCAAGAGAGGCACTTTAGAGCAAATCATGAAAGATCGATGGATGAATGTGGGTCACGAAGATGATGAACTAAAGCCTTACGTGGAGCCACTCCCTGACTACAAGGACCCCCGGCGGACAGAGCTGATGGTGTCCATGGGTTATACACGGGAAGAGATCCAGGACTCGCTGGTGGGCCAGAGATACAACGAGGTGATGGCCACCTATCTGCTCCTGGGCTAC</t>
   </si>
   <si>
@@ -662,12 +689,24 @@
     <t>D09</t>
   </si>
   <si>
+    <t>D10</t>
+  </si>
+  <si>
     <t>D11</t>
   </si>
   <si>
     <t>D12</t>
   </si>
   <si>
+    <t>D2</t>
+  </si>
+  <si>
+    <t>D3</t>
+  </si>
+  <si>
+    <t>D4</t>
+  </si>
+  <si>
     <t>DAPK1_HUMAN_D0</t>
   </si>
   <si>
@@ -725,15 +764,36 @@
     <t>E07</t>
   </si>
   <si>
+    <t>E1</t>
+  </si>
+  <si>
     <t>E10</t>
   </si>
   <si>
+    <t>E11</t>
+  </si>
+  <si>
     <t>E12</t>
   </si>
   <si>
     <t>E2AK2_HUMAN_D0</t>
   </si>
   <si>
+    <t>E3</t>
+  </si>
+  <si>
+    <t>E4</t>
+  </si>
+  <si>
+    <t>E5</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>E9</t>
+  </si>
+  <si>
     <t>EAFLTQKAKVGELKDDDFERISELGAGNGGVVTKVQHRPSGLIMARKLIHLEIKPAIRNQIIRELQVLHECNSPYIVGFYGAFYSDGEISICMEHMDGGSLDQVLKEAKRIPEEILGKVSIAVLRGLAYLREKHQIMHRDVKPSNILVNSRGEIKLCDFGVSGQLIDSMANSFVGTRSYMAPERLQGTHYSVQSDIWSMGLSLVELAVGRYPIPPPDAKELEAIFGRPVVDGEEGEPHSISPRPRPPGRPVSGHGMDSRPAMAIFELLDYIVNEPPPKLPNGVFTPDFQEFVNKCLIKNPAERADLKMLTNHTFIKRSEVEEVDFAGWLCKTLRLNQPGTPTRTAV</t>
   </si>
   <si>
@@ -770,12 +830,24 @@
     <t>F01</t>
   </si>
   <si>
+    <t>F1</t>
+  </si>
+  <si>
     <t>F11</t>
   </si>
   <si>
     <t>F12</t>
   </si>
   <si>
+    <t>F5</t>
+  </si>
+  <si>
+    <t>F6</t>
+  </si>
+  <si>
+    <t>F8</t>
+  </si>
+  <si>
     <t>FAK1_HUMAN_D0</t>
   </si>
   <si>
@@ -806,6 +878,12 @@
     <t>G07</t>
   </si>
   <si>
+    <t>G10</t>
+  </si>
+  <si>
+    <t>G5</t>
+  </si>
+  <si>
     <t>GAAACAAAGTATACTGTGGACAAGAGGTTTGGCATGGATTTTAAAGAAATAGAATTAATTGGCTCAGGTGGATTTGGCCAAGTTTTCAAAGCAAAACACAGAATTGACGGAAAGACTTACGTTATTAAACGTGTTAAATATAATAACGAGAAGGCGGAGCGTGAAGTAAAAGCATTGGCAAAACTTGATCATGTAAATATTGTTCACTACAATGGCTGTTGGGATGGATTTGATTATGATCCTGAGACCAGTGATGATTCTCTTGAGAGCAGTGATTATGATCCTGAGAACAGCAAAAATAGTTCAAGGTCAAAGACTAAGTGCCTTTTCATCCAAATGGAATTCTGTGATAAAGGGACCTTGGAACAATGGATTGAAAAAAGAAGAGGCGAGAAACTAGACAAAGTTTTGGCTTTGGAACTCTTTGAACAAATAACAAAAGGGGTGGATTATATACATTCAAAAAAATTAATTCATAGAGATCTTAAGCCAAGTAATATATTCTTAGTAGATACAAAACAAGTAAAGATTGGAGACTTTGGACTTGTAACATCTCTGAAAAATGATGGAAAGCGAACAAGGAGTAAGGGAACTTTGCGATACATGAGCCCAGAACAGATTTCTTCGCAAGACTATGGAAAGGAAGTGGACCTCTACGCTTTGGGGCTAATTCTTGCTGAACTTCTTCATGTATGTGACACTGCTTTTGAAACATCAAAGTTTTTCACAGACCTACGGGATGGCATCATCTCAGATATATTTGATAAAAAAGAAAAAACTCTTCTACAGAAATTACTCTCAAAGAAACCTGAGGATCGACCTAACACATCTGAAATACTAAGGACCTTGACTGTGTGGAAGAAAAGCCCAGAGAAAAATGAACGACACACATGT</t>
   </si>
   <si>
@@ -924,6 +1002,24 @@
   </si>
   <si>
     <t>H03</t>
+  </si>
+  <si>
+    <t>H1</t>
+  </si>
+  <si>
+    <t>H12</t>
+  </si>
+  <si>
+    <t>H3</t>
+  </si>
+  <si>
+    <t>H4</t>
+  </si>
+  <si>
+    <t>H5</t>
+  </si>
+  <si>
+    <t>H9</t>
   </si>
   <si>
     <t>HASP_HUMAN_D0</t>
@@ -1895,57 +1991,57 @@
   <sheetData>
     <row spans="1:12" r="1">
       <c t="s" r="A1">
-        <v>505</v>
+        <v>537</v>
       </c>
       <c t="s" r="B1">
-        <v>503</v>
+        <v>535</v>
       </c>
       <c t="s" r="C1">
-        <v>502</v>
+        <v>534</v>
       </c>
       <c t="s" r="D1">
-        <v>504</v>
+        <v>536</v>
       </c>
       <c t="s" r="E1">
-        <v>506</v>
+        <v>538</v>
       </c>
       <c t="s" r="F1">
-        <v>495</v>
+        <v>527</v>
       </c>
       <c t="s" r="G1">
-        <v>494</v>
+        <v>526</v>
       </c>
       <c t="s" r="H1">
-        <v>500</v>
+        <v>532</v>
       </c>
       <c t="s" r="I1">
-        <v>499</v>
+        <v>531</v>
       </c>
       <c t="s" r="J1">
-        <v>497</v>
+        <v>529</v>
       </c>
       <c t="s" r="K1">
-        <v>498</v>
+        <v>530</v>
       </c>
       <c t="s" r="L1">
-        <v>501</v>
+        <v>533</v>
       </c>
     </row>
     <row spans="1:12" r="2">
       <c t="s" r="A2">
-        <v>390</v>
+        <v>422</v>
       </c>
       <c t="s" r="B2">
-        <v>306</v>
+        <v>338</v>
       </c>
       <c t="s" r="C2">
-        <v>310</v>
+        <v>342</v>
       </c>
       <c t="s" r="D2">
-        <v>334</v>
+        <v>366</v>
       </c>
       <c t="s" r="E2">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c t="n" r="F2">
         <v>72</v>
@@ -1960,30 +2056,30 @@
         <v>1155</v>
       </c>
       <c t="s" r="J2">
-        <v>477</v>
+        <v>509</v>
       </c>
       <c t="s" r="K2">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c t="s" r="L2">
-        <v>133</v>
+        <v>135</v>
       </c>
     </row>
     <row spans="1:12" r="3">
       <c t="s" r="A3">
-        <v>407</v>
+        <v>439</v>
       </c>
       <c t="s" r="B3">
-        <v>306</v>
+        <v>338</v>
       </c>
       <c t="s" r="C3">
-        <v>315</v>
+        <v>347</v>
       </c>
       <c t="s" r="D3">
-        <v>336</v>
+        <v>368</v>
       </c>
       <c t="s" r="E3">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c t="n" r="F3">
         <v>1</v>
@@ -1998,30 +2094,30 @@
         <v>813</v>
       </c>
       <c t="s" r="J3">
-        <v>395</v>
+        <v>427</v>
       </c>
       <c t="s" r="K3">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c t="s" r="L3">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row spans="1:12" r="4">
       <c t="s" r="A4">
-        <v>253</v>
+        <v>277</v>
       </c>
       <c t="s" r="B4">
-        <v>306</v>
+        <v>338</v>
       </c>
       <c t="s" r="C4">
-        <v>322</v>
+        <v>354</v>
       </c>
       <c t="s" r="D4">
-        <v>336</v>
+        <v>368</v>
       </c>
       <c t="s" r="E4">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c t="n" r="F4">
         <v>411</v>
@@ -2036,30 +2132,30 @@
         <v>2067</v>
       </c>
       <c t="s" r="J4">
-        <v>464</v>
+        <v>496</v>
       </c>
       <c t="s" r="K4">
-        <v>468</v>
+        <v>500</v>
       </c>
       <c t="s" r="L4">
-        <v>100</v>
+        <v>102</v>
       </c>
     </row>
     <row spans="1:12" r="5">
       <c t="s" r="A5">
-        <v>389</v>
+        <v>421</v>
       </c>
       <c t="s" r="B5">
-        <v>306</v>
+        <v>338</v>
       </c>
       <c t="s" r="C5">
-        <v>329</v>
+        <v>361</v>
       </c>
       <c t="s" r="D5">
-        <v>335</v>
+        <v>367</v>
       </c>
       <c t="s" r="E5">
-        <v>261</v>
+        <v>285</v>
       </c>
       <c t="n" r="F5">
         <v>37</v>
@@ -2074,30 +2170,30 @@
         <v>1146</v>
       </c>
       <c t="s" r="J5">
-        <v>478</v>
+        <v>510</v>
       </c>
       <c t="s" r="K5">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c t="s" r="L5">
-        <v>131</v>
+        <v>133</v>
       </c>
     </row>
     <row spans="1:12" r="6">
       <c t="s" r="A6">
-        <v>165</v>
+        <v>170</v>
       </c>
       <c t="s" r="B6">
-        <v>306</v>
+        <v>338</v>
       </c>
       <c t="s" r="C6">
-        <v>320</v>
+        <v>352</v>
       </c>
       <c t="s" r="D6">
-        <v>337</v>
+        <v>369</v>
       </c>
       <c t="s" r="E6">
-        <v>259</v>
+        <v>283</v>
       </c>
       <c t="n" r="F6">
         <v>444</v>
@@ -2112,30 +2208,30 @@
         <v>2157</v>
       </c>
       <c t="s" r="J6">
-        <v>437</v>
+        <v>469</v>
       </c>
       <c t="s" r="K6">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c t="s" r="L6">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row spans="1:12" r="7">
       <c t="s" r="A7">
-        <v>217</v>
+        <v>230</v>
       </c>
       <c t="s" r="B7">
-        <v>306</v>
+        <v>338</v>
       </c>
       <c t="s" r="C7">
-        <v>321</v>
+        <v>353</v>
       </c>
       <c t="s" r="D7">
-        <v>339</v>
+        <v>371</v>
       </c>
       <c t="s" r="E7">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c t="n" r="F7">
         <v>2</v>
@@ -2150,27 +2246,27 @@
         <v>855</v>
       </c>
       <c t="s" r="J7">
-        <v>483</v>
+        <v>515</v>
       </c>
       <c t="s" r="K7">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c t="s" r="L7">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row spans="1:12" r="8">
       <c t="s" r="A8">
-        <v>404</v>
+        <v>436</v>
       </c>
       <c t="s" r="B8">
-        <v>306</v>
+        <v>338</v>
       </c>
       <c t="s" r="C8">
-        <v>328</v>
+        <v>360</v>
       </c>
       <c t="s" r="D8">
-        <v>337</v>
+        <v>369</v>
       </c>
       <c t="s" r="E8">
         <v>0</v>
@@ -2188,30 +2284,30 @@
         <v>891</v>
       </c>
       <c t="s" r="J8">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c t="s" r="K8">
-        <v>281</v>
+        <v>307</v>
       </c>
       <c t="s" r="L8">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row spans="1:12" r="9">
       <c t="s" r="A9">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c t="s" r="B9">
-        <v>306</v>
+        <v>338</v>
       </c>
       <c t="s" r="C9">
-        <v>319</v>
+        <v>351</v>
       </c>
       <c t="s" r="D9">
-        <v>336</v>
+        <v>368</v>
       </c>
       <c t="s" r="E9">
-        <v>252</v>
+        <v>273</v>
       </c>
       <c t="n" r="F9">
         <v>254</v>
@@ -2226,30 +2322,30 @@
         <v>1653</v>
       </c>
       <c t="s" r="J9">
-        <v>247</v>
+        <v>267</v>
       </c>
       <c t="s" r="K9">
-        <v>263</v>
+        <v>289</v>
       </c>
       <c t="s" r="L9">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row spans="1:12" r="10">
       <c t="s" r="A10">
-        <v>243</v>
+        <v>263</v>
       </c>
       <c t="s" r="B10">
-        <v>306</v>
+        <v>338</v>
       </c>
       <c t="s" r="C10">
-        <v>325</v>
+        <v>357</v>
       </c>
       <c t="s" r="D10">
-        <v>333</v>
+        <v>365</v>
       </c>
       <c t="s" r="E10">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c t="n" r="F10">
         <v>604</v>
@@ -2264,30 +2360,30 @@
         <v>2694</v>
       </c>
       <c t="s" r="J10">
-        <v>223</v>
+        <v>236</v>
       </c>
       <c t="s" r="K10">
-        <v>267</v>
+        <v>293</v>
       </c>
       <c t="s" r="L10">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row spans="1:12" r="11">
       <c t="s" r="A11">
-        <v>244</v>
+        <v>264</v>
       </c>
       <c t="s" r="B11">
-        <v>306</v>
+        <v>338</v>
       </c>
       <c t="s" r="C11">
-        <v>331</v>
+        <v>363</v>
       </c>
       <c t="s" r="D11">
-        <v>338</v>
+        <v>370</v>
       </c>
       <c t="s" r="E11">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c t="n" r="F11">
         <v>616</v>
@@ -2302,30 +2398,30 @@
         <v>2730</v>
       </c>
       <c t="s" r="J11">
-        <v>224</v>
+        <v>237</v>
       </c>
       <c t="s" r="K11">
-        <v>269</v>
+        <v>295</v>
       </c>
       <c t="s" r="L11">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row spans="1:12" r="12">
       <c t="s" r="A12">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c t="s" r="B12">
-        <v>306</v>
+        <v>338</v>
       </c>
       <c t="s" r="C12">
-        <v>327</v>
+        <v>359</v>
       </c>
       <c t="s" r="D12">
-        <v>336</v>
+        <v>368</v>
       </c>
       <c t="s" r="E12">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c t="n" r="F12">
         <v>229</v>
@@ -2340,30 +2436,30 @@
         <v>1536</v>
       </c>
       <c t="s" r="J12">
-        <v>450</v>
+        <v>482</v>
       </c>
       <c t="s" r="K12">
-        <v>472</v>
+        <v>504</v>
       </c>
       <c t="s" r="L12">
-        <v>151</v>
+        <v>153</v>
       </c>
     </row>
     <row spans="1:12" r="13">
       <c t="s" r="A13">
-        <v>359</v>
+        <v>391</v>
       </c>
       <c t="s" r="B13">
-        <v>306</v>
+        <v>338</v>
       </c>
       <c t="s" r="C13">
-        <v>330</v>
+        <v>362</v>
       </c>
       <c t="s" r="D13">
-        <v>334</v>
+        <v>366</v>
       </c>
       <c t="s" r="E13">
-        <v>251</v>
+        <v>272</v>
       </c>
       <c t="n" r="F13">
         <v>659</v>
@@ -2378,30 +2474,30 @@
         <v>2853</v>
       </c>
       <c t="s" r="J13">
-        <v>440</v>
+        <v>472</v>
       </c>
       <c t="s" r="K13">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c t="s" r="L13">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row spans="1:12" r="14">
       <c t="s" r="A14">
-        <v>457</v>
+        <v>489</v>
       </c>
       <c t="s" r="B14">
-        <v>306</v>
+        <v>338</v>
       </c>
       <c t="s" r="C14">
-        <v>312</v>
+        <v>344</v>
       </c>
       <c t="s" r="D14">
-        <v>335</v>
+        <v>367</v>
       </c>
       <c t="s" r="E14">
-        <v>250</v>
+        <v>270</v>
       </c>
       <c t="n" r="F14">
         <v>18</v>
@@ -2416,30 +2512,30 @@
         <v>951</v>
       </c>
       <c t="s" r="J14">
-        <v>438</v>
+        <v>470</v>
       </c>
       <c t="s" r="K14">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c t="s" r="L14">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row spans="1:12" r="15">
       <c t="s" r="A15">
-        <v>358</v>
+        <v>390</v>
       </c>
       <c t="s" r="B15">
-        <v>306</v>
+        <v>338</v>
       </c>
       <c t="s" r="C15">
-        <v>313</v>
+        <v>345</v>
       </c>
       <c t="s" r="D15">
-        <v>334</v>
+        <v>366</v>
       </c>
       <c t="s" r="E15">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c t="n" r="F15">
         <v>46</v>
@@ -2454,30 +2550,30 @@
         <v>1038</v>
       </c>
       <c t="s" r="J15">
-        <v>447</v>
+        <v>479</v>
       </c>
       <c t="s" r="K15">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c t="s" r="L15">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row spans="1:12" r="16">
       <c t="s" r="A16">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c t="s" r="B16">
-        <v>306</v>
+        <v>338</v>
       </c>
       <c t="s" r="C16">
-        <v>309</v>
+        <v>341</v>
       </c>
       <c t="s" r="D16">
-        <v>334</v>
+        <v>366</v>
       </c>
       <c t="s" r="E16">
-        <v>235</v>
+        <v>248</v>
       </c>
       <c t="n" r="F16">
         <v>1</v>
@@ -2492,30 +2588,30 @@
         <v>1002</v>
       </c>
       <c t="s" r="J16">
-        <v>394</v>
+        <v>426</v>
       </c>
       <c t="s" r="K16">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c t="s" r="L16">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row spans="1:12" r="17">
       <c t="s" r="A17">
-        <v>410</v>
+        <v>442</v>
       </c>
       <c t="s" r="B17">
-        <v>306</v>
+        <v>338</v>
       </c>
       <c t="s" r="C17">
-        <v>326</v>
+        <v>358</v>
       </c>
       <c t="s" r="D17">
-        <v>335</v>
+        <v>367</v>
       </c>
       <c t="s" r="E17">
-        <v>236</v>
+        <v>250</v>
       </c>
       <c t="n" r="F17">
         <v>248</v>
@@ -2530,30 +2626,30 @@
         <v>1635</v>
       </c>
       <c t="s" r="J17">
-        <v>397</v>
+        <v>429</v>
       </c>
       <c t="s" r="K17">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c t="s" r="L17">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row spans="1:12" r="18">
       <c t="s" r="A18">
-        <v>392</v>
+        <v>424</v>
       </c>
       <c t="s" r="B18">
-        <v>306</v>
+        <v>338</v>
       </c>
       <c t="s" r="C18">
-        <v>318</v>
+        <v>350</v>
       </c>
       <c t="s" r="D18">
-        <v>336</v>
+        <v>368</v>
       </c>
       <c t="s" r="E18">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c t="n" r="F18">
         <v>80</v>
@@ -2568,30 +2664,30 @@
         <v>1197</v>
       </c>
       <c t="s" r="J18">
-        <v>446</v>
+        <v>478</v>
       </c>
       <c t="s" r="K18">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c t="s" r="L18">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row spans="1:12" r="19">
       <c t="s" r="A19">
-        <v>367</v>
+        <v>399</v>
       </c>
       <c t="s" r="B19">
-        <v>306</v>
+        <v>338</v>
       </c>
       <c t="s" r="C19">
-        <v>316</v>
+        <v>348</v>
       </c>
       <c t="s" r="D19">
-        <v>336</v>
+        <v>368</v>
       </c>
       <c t="s" r="E19">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c t="n" r="F19">
         <v>16</v>
@@ -2606,30 +2702,30 @@
         <v>990</v>
       </c>
       <c t="s" r="J19">
-        <v>305</v>
+        <v>337</v>
       </c>
       <c t="s" r="K19">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c t="s" r="L19">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row spans="1:12" r="20">
       <c t="s" r="A20">
-        <v>382</v>
+        <v>414</v>
       </c>
       <c t="s" r="B20">
-        <v>306</v>
+        <v>338</v>
       </c>
       <c t="s" r="C20">
-        <v>317</v>
+        <v>349</v>
       </c>
       <c t="s" r="D20">
-        <v>335</v>
+        <v>367</v>
       </c>
       <c t="s" r="E20">
-        <v>233</v>
+        <v>246</v>
       </c>
       <c t="n" r="F20">
         <v>1</v>
@@ -2644,30 +2740,30 @@
         <v>1080</v>
       </c>
       <c t="s" r="J20">
-        <v>360</v>
+        <v>392</v>
       </c>
       <c t="s" r="K20">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c t="s" r="L20">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row spans="1:12" r="21">
       <c t="s" r="A21">
-        <v>384</v>
+        <v>416</v>
       </c>
       <c t="s" r="B21">
-        <v>306</v>
+        <v>338</v>
       </c>
       <c t="s" r="C21">
-        <v>314</v>
+        <v>346</v>
       </c>
       <c t="s" r="D21">
-        <v>332</v>
+        <v>364</v>
       </c>
       <c t="s" r="E21">
-        <v>166</v>
+        <v>171</v>
       </c>
       <c t="n" r="F21">
         <v>1</v>
@@ -2682,30 +2778,30 @@
         <v>1089</v>
       </c>
       <c t="s" r="J21">
-        <v>402</v>
+        <v>434</v>
       </c>
       <c t="s" r="K21">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c t="s" r="L21">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row spans="1:12" r="22">
       <c t="s" r="A22">
-        <v>463</v>
+        <v>495</v>
       </c>
       <c t="s" r="B22">
-        <v>306</v>
+        <v>338</v>
       </c>
       <c t="s" r="C22">
-        <v>311</v>
+        <v>343</v>
       </c>
       <c t="s" r="D22">
-        <v>338</v>
+        <v>370</v>
       </c>
       <c t="s" r="E22">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c t="n" r="F22">
         <v>30</v>
@@ -2720,30 +2816,30 @@
         <v>1206</v>
       </c>
       <c t="s" r="J22">
-        <v>403</v>
+        <v>435</v>
       </c>
       <c t="s" r="K22">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c t="s" r="L22">
-        <v>136</v>
+        <v>138</v>
       </c>
     </row>
     <row spans="1:12" r="23">
       <c t="s" r="A23">
-        <v>374</v>
+        <v>406</v>
       </c>
       <c t="s" r="B23">
-        <v>306</v>
+        <v>338</v>
       </c>
       <c t="s" r="C23">
-        <v>324</v>
+        <v>356</v>
       </c>
       <c t="s" r="D23">
-        <v>338</v>
+        <v>370</v>
       </c>
       <c t="s" r="E23">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c t="n" r="F23">
         <v>1</v>
@@ -2758,30 +2854,30 @@
         <v>978</v>
       </c>
       <c t="s" r="J23">
-        <v>388</v>
+        <v>420</v>
       </c>
       <c t="s" r="K23">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c t="s" r="L23">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row spans="1:12" r="24">
       <c t="s" r="A24">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c t="s" r="B24">
-        <v>306</v>
+        <v>338</v>
       </c>
       <c t="s" r="C24">
-        <v>323</v>
+        <v>355</v>
       </c>
       <c t="s" r="D24">
-        <v>339</v>
+        <v>371</v>
       </c>
       <c t="s" r="E24">
-        <v>301</v>
+        <v>327</v>
       </c>
       <c t="n" r="F24">
         <v>1</v>
@@ -2796,30 +2892,30 @@
         <v>1020</v>
       </c>
       <c t="s" r="J24">
-        <v>362</v>
+        <v>394</v>
       </c>
       <c t="s" r="K24">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c t="s" r="L24">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row spans="1:12" r="25">
       <c t="s" r="A25">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c t="s" r="B25">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c t="s" r="C25">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c t="s" r="D25">
-        <v>429</v>
+        <v>461</v>
       </c>
       <c t="s" r="E25">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c t="n" r="F25">
         <v>2</v>
@@ -2834,30 +2930,30 @@
         <v>1014</v>
       </c>
       <c t="s" r="J25">
-        <v>307</v>
+        <v>339</v>
       </c>
       <c t="s" r="K25">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c t="s" r="L25">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row spans="1:12" r="26">
       <c t="s" r="A26">
-        <v>303</v>
+        <v>335</v>
       </c>
       <c t="s" r="B26">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c t="s" r="C26">
-        <v>294</v>
+        <v>320</v>
       </c>
       <c t="s" r="D26">
-        <v>426</v>
+        <v>458</v>
       </c>
       <c t="s" r="E26">
-        <v>169</v>
+        <v>174</v>
       </c>
       <c t="n" r="F26">
         <v>24</v>
@@ -2872,30 +2968,30 @@
         <v>1071</v>
       </c>
       <c t="s" r="J26">
-        <v>283</v>
+        <v>309</v>
       </c>
       <c t="s" r="K26">
-        <v>284</v>
+        <v>310</v>
       </c>
       <c t="s" r="L26">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row spans="1:12" r="27">
       <c t="s" r="A27">
-        <v>393</v>
+        <v>425</v>
       </c>
       <c t="s" r="B27">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c t="s" r="C27">
-        <v>363</v>
+        <v>395</v>
       </c>
       <c t="s" r="D27">
-        <v>427</v>
+        <v>459</v>
       </c>
       <c t="s" r="E27">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c t="n" r="F27">
         <v>2</v>
@@ -2910,30 +3006,30 @@
         <v>867</v>
       </c>
       <c t="s" r="J27">
-        <v>249</v>
+        <v>269</v>
       </c>
       <c t="s" r="K27">
-        <v>272</v>
+        <v>298</v>
       </c>
       <c t="s" r="L27">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row spans="1:12" r="28">
       <c t="s" r="A28">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c t="s" r="B28">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c t="s" r="C28">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c t="s" r="D28">
-        <v>428</v>
+        <v>460</v>
       </c>
       <c t="s" r="E28">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c t="n" r="F28">
         <v>2</v>
@@ -2948,30 +3044,30 @@
         <v>912</v>
       </c>
       <c t="s" r="J28">
-        <v>372</v>
+        <v>404</v>
       </c>
       <c t="s" r="K28">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c t="s" r="L28">
-        <v>44</v>
+        <v>46</v>
       </c>
     </row>
     <row spans="1:12" r="29">
       <c t="s" r="A29">
-        <v>164</v>
+        <v>169</v>
       </c>
       <c t="s" r="B29">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c t="s" r="C29">
-        <v>163</v>
+        <v>168</v>
       </c>
       <c t="s" r="D29">
-        <v>426</v>
+        <v>458</v>
       </c>
       <c t="s" r="E29">
-        <v>301</v>
+        <v>327</v>
       </c>
       <c t="n" r="F29">
         <v>1</v>
@@ -2986,30 +3082,30 @@
         <v>987</v>
       </c>
       <c t="s" r="J29">
-        <v>370</v>
+        <v>402</v>
       </c>
       <c t="s" r="K29">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c t="s" r="L29">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row spans="1:12" r="30">
       <c t="s" r="A30">
-        <v>344</v>
+        <v>376</v>
       </c>
       <c t="s" r="B30">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c t="s" r="C30">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c t="s" r="D30">
-        <v>426</v>
+        <v>458</v>
       </c>
       <c t="s" r="E30">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c t="n" r="F30">
         <v>24</v>
@@ -3024,30 +3120,30 @@
         <v>993</v>
       </c>
       <c t="s" r="J30">
-        <v>441</v>
+        <v>473</v>
       </c>
       <c t="s" r="K30">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c t="s" r="L30">
-        <v>49</v>
+        <v>51</v>
       </c>
     </row>
     <row spans="1:12" r="31">
       <c t="s" r="A31">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c t="s" r="B31">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c t="s" r="C31">
-        <v>228</v>
+        <v>241</v>
       </c>
       <c t="s" r="D31">
-        <v>426</v>
+        <v>458</v>
       </c>
       <c t="s" r="E31">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c t="n" r="F31">
         <v>24</v>
@@ -3062,30 +3158,30 @@
         <v>1146</v>
       </c>
       <c t="s" r="J31">
-        <v>454</v>
+        <v>486</v>
       </c>
       <c t="s" r="K31">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c t="s" r="L31">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row spans="1:12" r="32">
       <c t="s" r="A32">
-        <v>345</v>
+        <v>377</v>
       </c>
       <c t="s" r="B32">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c t="s" r="C32">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c t="s" r="D32">
-        <v>429</v>
+        <v>461</v>
       </c>
       <c t="s" r="E32">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c t="n" r="F32">
         <v>4</v>
@@ -3100,27 +3196,27 @@
         <v>936</v>
       </c>
       <c t="s" r="J32">
-        <v>409</v>
+        <v>441</v>
       </c>
       <c t="s" r="K32">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c t="s" r="L32">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row spans="1:12" r="33">
       <c t="s" r="A33">
-        <v>459</v>
+        <v>491</v>
       </c>
       <c t="s" r="B33">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c t="s" r="C33">
-        <v>458</v>
+        <v>490</v>
       </c>
       <c t="s" r="D33">
-        <v>429</v>
+        <v>461</v>
       </c>
       <c t="s" r="E33">
         <v>1</v>
@@ -3138,30 +3234,30 @@
         <v>948</v>
       </c>
       <c t="s" r="J33">
-        <v>487</v>
+        <v>519</v>
       </c>
       <c t="s" r="K33">
-        <v>295</v>
+        <v>321</v>
       </c>
       <c t="s" r="L33">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row spans="1:12" r="34">
       <c t="s" r="A34">
-        <v>481</v>
+        <v>513</v>
       </c>
       <c t="s" r="B34">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c t="s" r="C34">
-        <v>480</v>
+        <v>512</v>
       </c>
       <c t="s" r="D34">
-        <v>426</v>
+        <v>458</v>
       </c>
       <c t="s" r="E34">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c t="n" r="F34">
         <v>24</v>
@@ -3176,30 +3272,30 @@
         <v>939</v>
       </c>
       <c t="s" r="J34">
-        <v>465</v>
+        <v>497</v>
       </c>
       <c t="s" r="K34">
-        <v>473</v>
+        <v>505</v>
       </c>
       <c t="s" r="L34">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row spans="1:12" r="35">
       <c t="s" r="A35">
-        <v>348</v>
+        <v>380</v>
       </c>
       <c t="s" r="B35">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c t="s" r="C35">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c t="s" r="D35">
-        <v>426</v>
+        <v>458</v>
       </c>
       <c t="s" r="E35">
-        <v>300</v>
+        <v>326</v>
       </c>
       <c t="n" r="F35">
         <v>24</v>
@@ -3214,30 +3310,30 @@
         <v>939</v>
       </c>
       <c t="s" r="J35">
-        <v>493</v>
+        <v>525</v>
       </c>
       <c t="s" r="K35">
-        <v>467</v>
+        <v>499</v>
       </c>
       <c t="s" r="L35">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row spans="1:12" r="36">
       <c t="s" r="A36">
-        <v>490</v>
+        <v>522</v>
       </c>
       <c t="s" r="B36">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c t="s" r="C36">
-        <v>489</v>
+        <v>521</v>
       </c>
       <c t="s" r="D36">
-        <v>426</v>
+        <v>458</v>
       </c>
       <c t="s" r="E36">
-        <v>231</v>
+        <v>244</v>
       </c>
       <c t="n" r="F36">
         <v>24</v>
@@ -3252,30 +3348,30 @@
         <v>1035</v>
       </c>
       <c t="s" r="J36">
-        <v>416</v>
+        <v>448</v>
       </c>
       <c t="s" r="K36">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c t="s" r="L36">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row spans="1:12" r="37">
       <c t="s" r="A37">
-        <v>492</v>
+        <v>524</v>
       </c>
       <c t="s" r="B37">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c t="s" r="C37">
-        <v>491</v>
+        <v>523</v>
       </c>
       <c t="s" r="D37">
-        <v>426</v>
+        <v>458</v>
       </c>
       <c t="s" r="E37">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c t="n" r="F37">
         <v>24</v>
@@ -3290,30 +3386,30 @@
         <v>1056</v>
       </c>
       <c t="s" r="J37">
-        <v>482</v>
+        <v>514</v>
       </c>
       <c t="s" r="K37">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c t="s" r="L37">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row spans="1:12" r="38">
       <c t="s" r="A38">
-        <v>423</v>
+        <v>455</v>
       </c>
       <c t="s" r="B38">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c t="s" r="C38">
-        <v>420</v>
+        <v>452</v>
       </c>
       <c t="s" r="D38">
-        <v>427</v>
+        <v>459</v>
       </c>
       <c t="s" r="E38">
-        <v>262</v>
+        <v>286</v>
       </c>
       <c t="n" r="F38">
         <v>24</v>
@@ -3328,30 +3424,30 @@
         <v>933</v>
       </c>
       <c t="s" r="J38">
-        <v>308</v>
+        <v>340</v>
       </c>
       <c t="s" r="K38">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c t="s" r="L38">
-        <v>50</v>
+        <v>52</v>
       </c>
     </row>
     <row spans="1:12" r="39">
       <c t="s" r="A39">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c t="s" r="B39">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c t="s" r="C39">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c t="s" r="D39">
-        <v>425</v>
+        <v>457</v>
       </c>
       <c t="s" r="E39">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c t="n" r="F39">
         <v>24</v>
@@ -3366,30 +3462,30 @@
         <v>1143</v>
       </c>
       <c t="s" r="J39">
-        <v>433</v>
+        <v>465</v>
       </c>
       <c t="s" r="K39">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c t="s" r="L39">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row spans="1:12" r="40">
       <c t="s" r="A40">
-        <v>274</v>
+        <v>300</v>
       </c>
       <c t="s" r="B40">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c t="s" r="C40">
-        <v>273</v>
+        <v>299</v>
       </c>
       <c t="s" r="D40">
-        <v>427</v>
+        <v>459</v>
       </c>
       <c t="s" r="E40">
-        <v>237</v>
+        <v>252</v>
       </c>
       <c t="n" r="F40">
         <v>24</v>
@@ -3404,30 +3500,30 @@
         <v>1077</v>
       </c>
       <c t="s" r="J40">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c t="s" r="K40">
-        <v>280</v>
+        <v>306</v>
       </c>
       <c t="s" r="L40">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row spans="1:12" r="41">
       <c t="s" r="A41">
-        <v>414</v>
+        <v>446</v>
       </c>
       <c t="s" r="B41">
+        <v>476</v>
+      </c>
+      <c t="s" r="C41">
         <v>444</v>
       </c>
-      <c t="s" r="C41">
-        <v>412</v>
-      </c>
       <c t="s" r="D41">
-        <v>425</v>
+        <v>457</v>
       </c>
       <c t="s" r="E41">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c t="n" r="F41">
         <v>24</v>
@@ -3442,30 +3538,30 @@
         <v>954</v>
       </c>
       <c t="s" r="J41">
-        <v>453</v>
+        <v>485</v>
       </c>
       <c t="s" r="K41">
-        <v>471</v>
+        <v>503</v>
       </c>
       <c t="s" r="L41">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row spans="1:12" r="42">
       <c t="s" r="A42">
-        <v>449</v>
+        <v>481</v>
       </c>
       <c t="s" r="B42">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c t="s" r="C42">
-        <v>448</v>
+        <v>480</v>
       </c>
       <c t="s" r="D42">
-        <v>426</v>
+        <v>458</v>
       </c>
       <c t="s" r="E42">
-        <v>260</v>
+        <v>284</v>
       </c>
       <c t="n" r="F42">
         <v>24</v>
@@ -3480,30 +3576,30 @@
         <v>975</v>
       </c>
       <c t="s" r="J42">
-        <v>355</v>
+        <v>387</v>
       </c>
       <c t="s" r="K42">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c t="s" r="L42">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
     <row spans="1:12" r="43">
       <c t="s" r="A43">
-        <v>456</v>
+        <v>488</v>
       </c>
       <c t="s" r="B43">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c t="s" r="C43">
-        <v>460</v>
+        <v>492</v>
       </c>
       <c t="s" r="D43">
-        <v>426</v>
+        <v>458</v>
       </c>
       <c t="s" r="E43">
-        <v>302</v>
+        <v>328</v>
       </c>
       <c t="n" r="F43">
         <v>23</v>
@@ -3518,30 +3614,30 @@
         <v>981</v>
       </c>
       <c t="s" r="J43">
-        <v>377</v>
+        <v>409</v>
       </c>
       <c t="s" r="K43">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c t="s" r="L43">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row spans="1:12" r="44">
       <c t="s" r="A44">
-        <v>352</v>
+        <v>384</v>
       </c>
       <c t="s" r="B44">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c t="s" r="C44">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c t="s" r="D44">
-        <v>427</v>
+        <v>459</v>
       </c>
       <c t="s" r="E44">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c t="n" r="F44">
         <v>2</v>
@@ -3556,27 +3652,27 @@
         <v>981</v>
       </c>
       <c t="s" r="J44">
-        <v>455</v>
+        <v>487</v>
       </c>
       <c t="s" r="K44">
-        <v>474</v>
+        <v>506</v>
       </c>
       <c t="s" r="L44">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row spans="1:12" r="45">
       <c t="s" r="A45">
-        <v>351</v>
+        <v>383</v>
       </c>
       <c t="s" r="B45">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c t="s" r="C45">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c t="s" r="D45">
-        <v>426</v>
+        <v>458</v>
       </c>
       <c t="s" r="E45">
         <v>2</v>
@@ -3594,30 +3690,30 @@
         <v>1002</v>
       </c>
       <c t="s" r="J45">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c t="s" r="K45">
-        <v>278</v>
+        <v>304</v>
       </c>
       <c t="s" r="L45">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row spans="1:12" r="46">
       <c t="s" r="A46">
-        <v>346</v>
+        <v>378</v>
       </c>
       <c t="s" r="B46">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c t="s" r="C46">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c t="s" r="D46">
-        <v>426</v>
+        <v>458</v>
       </c>
       <c t="s" r="E46">
-        <v>234</v>
+        <v>247</v>
       </c>
       <c t="n" r="F46">
         <v>24</v>
@@ -3632,30 +3728,30 @@
         <v>1053</v>
       </c>
       <c t="s" r="J46">
-        <v>298</v>
+        <v>324</v>
       </c>
       <c t="s" r="K46">
-        <v>286</v>
+        <v>312</v>
       </c>
       <c t="s" r="L46">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row spans="1:12" r="47">
       <c t="s" r="A47">
-        <v>385</v>
+        <v>417</v>
       </c>
       <c t="s" r="B47">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c t="s" r="C47">
-        <v>364</v>
+        <v>396</v>
       </c>
       <c t="s" r="D47">
-        <v>427</v>
+        <v>459</v>
       </c>
       <c t="s" r="E47">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c t="n" r="F47">
         <v>24</v>
@@ -3670,30 +3766,30 @@
         <v>1107</v>
       </c>
       <c t="s" r="J47">
-        <v>436</v>
+        <v>468</v>
       </c>
       <c t="s" r="K47">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c t="s" r="L47">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row spans="1:12" r="48">
       <c t="s" r="A48">
-        <v>357</v>
+        <v>389</v>
       </c>
       <c t="s" r="B48">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c t="s" r="C48">
-        <v>439</v>
+        <v>471</v>
       </c>
       <c t="s" r="D48">
-        <v>427</v>
+        <v>459</v>
       </c>
       <c t="s" r="E48">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c t="n" r="F48">
         <v>24</v>
@@ -3708,30 +3804,30 @@
         <v>1038</v>
       </c>
       <c t="s" r="J48">
-        <v>485</v>
+        <v>517</v>
       </c>
       <c t="s" r="K48">
-        <v>297</v>
+        <v>323</v>
       </c>
       <c t="s" r="L48">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row spans="1:12" r="49">
       <c t="s" r="A49">
-        <v>406</v>
+        <v>438</v>
       </c>
       <c t="s" r="B49">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c t="s" r="C49">
-        <v>405</v>
+        <v>437</v>
       </c>
       <c t="s" r="D49">
-        <v>428</v>
+        <v>460</v>
       </c>
       <c t="s" r="E49">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c t="n" r="F49">
         <v>23</v>
@@ -3746,27 +3842,27 @@
         <v>1050</v>
       </c>
       <c t="s" r="J49">
-        <v>373</v>
+        <v>405</v>
       </c>
       <c t="s" r="K49">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c t="s" r="L49">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row spans="1:12" r="50">
       <c t="s" r="A50">
-        <v>418</v>
+        <v>450</v>
       </c>
       <c t="s" r="B50">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c t="s" r="C50">
-        <v>417</v>
+        <v>449</v>
       </c>
       <c t="s" r="D50">
-        <v>428</v>
+        <v>460</v>
       </c>
       <c t="s" r="E50">
         <v>3</v>
@@ -3784,30 +3880,30 @@
         <v>1095</v>
       </c>
       <c t="s" r="J50">
-        <v>293</v>
+        <v>319</v>
       </c>
       <c t="s" r="K50">
-        <v>288</v>
+        <v>314</v>
       </c>
       <c t="s" r="L50">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row spans="1:12" r="51">
       <c t="s" r="A51">
-        <v>230</v>
+        <v>243</v>
       </c>
       <c t="s" r="B51">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c t="s" r="C51">
-        <v>229</v>
+        <v>242</v>
       </c>
       <c t="s" r="D51">
-        <v>428</v>
+        <v>460</v>
       </c>
       <c t="s" r="E51">
-        <v>216</v>
+        <v>226</v>
       </c>
       <c t="n" r="F51">
         <v>23</v>
@@ -3822,27 +3918,27 @@
         <v>1251</v>
       </c>
       <c t="s" r="J51">
-        <v>381</v>
+        <v>413</v>
       </c>
       <c t="s" r="K51">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c t="s" r="L51">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row spans="1:12" r="52">
       <c t="s" r="A52">
-        <v>221</v>
+        <v>234</v>
       </c>
       <c t="s" r="B52">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c t="s" r="C52">
-        <v>220</v>
+        <v>233</v>
       </c>
       <c t="s" r="D52">
-        <v>426</v>
+        <v>458</v>
       </c>
       <c t="s" r="E52">
         <v>1</v>
@@ -3860,30 +3956,30 @@
         <v>1299</v>
       </c>
       <c t="s" r="J52">
-        <v>432</v>
+        <v>464</v>
       </c>
       <c t="s" r="K52">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c t="s" r="L52">
-        <v>52</v>
+        <v>54</v>
       </c>
     </row>
     <row spans="1:12" r="53">
       <c t="s" r="A53">
-        <v>396</v>
+        <v>428</v>
       </c>
       <c t="s" r="B53">
-        <v>444</v>
+        <v>476</v>
       </c>
       <c t="s" r="C53">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c t="s" r="D53">
-        <v>428</v>
+        <v>460</v>
       </c>
       <c t="s" r="E53">
-        <v>215</v>
+        <v>225</v>
       </c>
       <c t="n" r="F53">
         <v>1</v>
@@ -3898,25 +3994,31 @@
         <v>1272</v>
       </c>
       <c t="s" r="J53">
-        <v>398</v>
+        <v>430</v>
       </c>
       <c t="s" r="K53">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c t="s" r="L53">
-        <v>146</v>
+        <v>148</v>
       </c>
     </row>
     <row spans="1:12" r="54">
       <c t="s" r="A54">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c t="s" r="B54">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C54">
         <v>23941</v>
       </c>
+      <c t="n" r="D54">
+        <v>6</v>
+      </c>
+      <c t="s" r="E54">
+        <v>276</v>
+      </c>
       <c t="n" r="F54">
         <v>186</v>
       </c>
@@ -3930,25 +4032,31 @@
         <v>1350</v>
       </c>
       <c t="s" r="J54">
-        <v>445</v>
+        <v>477</v>
       </c>
       <c t="s" r="K54">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c t="s" r="L54">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row spans="1:12" r="55">
       <c t="s" r="A55">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c t="s" r="B55">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C55">
         <v>23777</v>
       </c>
+      <c t="n" r="D55">
+        <v>5</v>
+      </c>
+      <c t="s" r="E55">
+        <v>255</v>
+      </c>
       <c t="n" r="F55">
         <v>1</v>
       </c>
@@ -3962,25 +4070,31 @@
         <v>891</v>
       </c>
       <c t="s" r="J55">
-        <v>378</v>
+        <v>410</v>
       </c>
       <c t="s" r="K55">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c t="s" r="L55">
-        <v>80</v>
+        <v>82</v>
       </c>
     </row>
     <row spans="1:12" r="56">
       <c t="s" r="A56">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c t="s" r="B56">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C56">
         <v>23688</v>
       </c>
+      <c t="n" r="D56">
+        <v>4</v>
+      </c>
+      <c t="s" r="E56">
+        <v>258</v>
+      </c>
       <c t="n" r="F56">
         <v>1</v>
       </c>
@@ -3994,25 +4108,31 @@
         <v>903</v>
       </c>
       <c t="s" r="J56">
-        <v>371</v>
+        <v>403</v>
       </c>
       <c t="s" r="K56">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c t="s" r="L56">
-        <v>82</v>
+        <v>84</v>
       </c>
     </row>
     <row spans="1:12" r="57">
       <c t="s" r="A57">
-        <v>218</v>
+        <v>231</v>
       </c>
       <c t="s" r="B57">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C57">
         <v>23436</v>
       </c>
+      <c t="n" r="D57">
+        <v>1</v>
+      </c>
+      <c t="s" r="E57">
+        <v>331</v>
+      </c>
       <c t="n" r="F57">
         <v>9</v>
       </c>
@@ -4026,25 +4146,31 @@
         <v>867</v>
       </c>
       <c t="s" r="J57">
-        <v>484</v>
+        <v>516</v>
       </c>
       <c t="s" r="K57">
-        <v>296</v>
+        <v>322</v>
       </c>
       <c t="s" r="L57">
-        <v>137</v>
+        <v>139</v>
       </c>
     </row>
     <row spans="1:12" r="58">
       <c t="s" r="A58">
-        <v>245</v>
+        <v>265</v>
       </c>
       <c t="s" r="B58">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C58">
         <v>23896</v>
       </c>
+      <c t="n" r="D58">
+        <v>6</v>
+      </c>
+      <c t="s" r="E58">
+        <v>164</v>
+      </c>
       <c t="n" r="F58">
         <v>598</v>
       </c>
@@ -4058,25 +4184,31 @@
         <v>2676</v>
       </c>
       <c t="s" r="J58">
-        <v>226</v>
+        <v>239</v>
       </c>
       <c t="s" r="K58">
-        <v>268</v>
+        <v>294</v>
       </c>
       <c t="s" r="L58">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row spans="1:12" r="59">
       <c t="s" r="A59">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c t="s" r="B59">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C59">
         <v>23532</v>
       </c>
+      <c t="n" r="D59">
+        <v>2</v>
+      </c>
+      <c t="s" r="E59">
+        <v>333</v>
+      </c>
       <c t="n" r="F59">
         <v>125</v>
       </c>
@@ -4090,25 +4222,31 @@
         <v>1173</v>
       </c>
       <c t="s" r="J59">
-        <v>356</v>
+        <v>388</v>
       </c>
       <c t="s" r="K59">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c t="s" r="L59">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row spans="1:12" r="60">
       <c t="s" r="A60">
-        <v>254</v>
+        <v>278</v>
       </c>
       <c t="s" r="B60">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C60">
         <v>23898</v>
       </c>
+      <c t="n" r="D60">
+        <v>6</v>
+      </c>
+      <c t="s" r="E60">
+        <v>177</v>
+      </c>
       <c t="n" r="F60">
         <v>414</v>
       </c>
@@ -4122,25 +4260,31 @@
         <v>2076</v>
       </c>
       <c t="s" r="J60">
-        <v>290</v>
+        <v>316</v>
       </c>
       <c t="s" r="K60">
-        <v>285</v>
+        <v>311</v>
       </c>
       <c t="s" r="L60">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row spans="1:12" r="61">
       <c t="s" r="A61">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c t="s" r="B61">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C61">
         <v>23671</v>
       </c>
+      <c t="n" r="D61">
+        <v>4</v>
+      </c>
+      <c t="s" r="E61">
+        <v>229</v>
+      </c>
       <c t="n" r="F61">
         <v>6</v>
       </c>
@@ -4154,25 +4298,31 @@
         <v>837</v>
       </c>
       <c t="s" r="J61">
-        <v>354</v>
+        <v>386</v>
       </c>
       <c t="s" r="K61">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c t="s" r="L61">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row spans="1:12" r="62">
       <c t="s" r="A62">
-        <v>257</v>
+        <v>281</v>
       </c>
       <c t="s" r="B62">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C62">
         <v>23904</v>
       </c>
+      <c t="n" r="D62">
+        <v>6</v>
+      </c>
+      <c t="s" r="E62">
+        <v>181</v>
+      </c>
       <c t="n" r="F62">
         <v>477</v>
       </c>
@@ -4186,25 +4336,31 @@
         <v>2361</v>
       </c>
       <c t="s" r="J62">
-        <v>422</v>
+        <v>454</v>
       </c>
       <c t="s" r="K62">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c t="s" r="L62">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row spans="1:12" r="63">
       <c t="s" r="A63">
-        <v>342</v>
+        <v>374</v>
       </c>
       <c t="s" r="B63">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C63">
         <v>23796</v>
       </c>
+      <c t="n" r="D63">
+        <v>5</v>
+      </c>
+      <c t="s" r="E63">
+        <v>272</v>
+      </c>
       <c t="n" r="F63">
         <v>1</v>
       </c>
@@ -4218,25 +4374,31 @@
         <v>882</v>
       </c>
       <c t="s" r="J63">
-        <v>376</v>
+        <v>408</v>
       </c>
       <c t="s" r="K63">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c t="s" r="L63">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row spans="1:12" r="64">
       <c t="s" r="A64">
-        <v>343</v>
+        <v>375</v>
       </c>
       <c t="s" r="B64">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C64">
         <v>23797</v>
       </c>
+      <c t="n" r="D64">
+        <v>5</v>
+      </c>
+      <c t="s" r="E64">
+        <v>273</v>
+      </c>
       <c t="n" r="F64">
         <v>1</v>
       </c>
@@ -4250,25 +4412,31 @@
         <v>882</v>
       </c>
       <c t="s" r="J64">
-        <v>375</v>
+        <v>407</v>
       </c>
       <c t="s" r="K64">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c t="s" r="L64">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row spans="1:12" r="65">
       <c t="s" r="A65">
-        <v>486</v>
+        <v>518</v>
       </c>
       <c t="s" r="B65">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C65">
         <v>23912</v>
       </c>
+      <c t="n" r="D65">
+        <v>6</v>
+      </c>
+      <c t="s" r="E65">
+        <v>228</v>
+      </c>
       <c t="n" r="F65">
         <v>801</v>
       </c>
@@ -4282,25 +4450,31 @@
         <v>3474</v>
       </c>
       <c t="s" r="J65">
-        <v>415</v>
+        <v>447</v>
       </c>
       <c t="s" r="K65">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c t="s" r="L65">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row spans="1:12" r="66">
       <c t="s" r="A66">
-        <v>256</v>
+        <v>280</v>
       </c>
       <c t="s" r="B66">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C66">
         <v>23922</v>
       </c>
+      <c t="n" r="D66">
+        <v>6</v>
+      </c>
+      <c t="s" r="E66">
+        <v>249</v>
+      </c>
       <c t="n" r="F66">
         <v>456</v>
       </c>
@@ -4314,25 +4488,31 @@
         <v>2289</v>
       </c>
       <c t="s" r="J66">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c t="s" r="K66">
-        <v>277</v>
+        <v>303</v>
       </c>
       <c t="s" r="L66">
-        <v>149</v>
+        <v>151</v>
       </c>
     </row>
     <row spans="1:12" r="67">
       <c t="s" r="A67">
-        <v>452</v>
+        <v>484</v>
       </c>
       <c t="s" r="B67">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C67">
         <v>23934</v>
       </c>
+      <c t="n" r="D67">
+        <v>6</v>
+      </c>
+      <c t="s" r="E67">
+        <v>271</v>
+      </c>
       <c t="n" r="F67">
         <v>254</v>
       </c>
@@ -4346,25 +4526,31 @@
         <v>1608</v>
       </c>
       <c t="s" r="J67">
-        <v>434</v>
+        <v>466</v>
       </c>
       <c t="s" r="K67">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c t="s" r="L67">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row spans="1:12" r="68">
       <c t="s" r="A68">
-        <v>242</v>
+        <v>262</v>
       </c>
       <c t="s" r="B68">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C68">
         <v>23930</v>
       </c>
+      <c t="n" r="D68">
+        <v>6</v>
+      </c>
+      <c t="s" r="E68">
+        <v>258</v>
+      </c>
       <c t="n" r="F68">
         <v>602</v>
       </c>
@@ -4378,25 +4564,31 @@
         <v>2688</v>
       </c>
       <c t="s" r="J68">
-        <v>225</v>
+        <v>238</v>
       </c>
       <c t="s" r="K68">
-        <v>275</v>
+        <v>301</v>
       </c>
       <c t="s" r="L68">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row spans="1:12" r="69">
       <c t="s" r="A69">
-        <v>349</v>
+        <v>381</v>
       </c>
       <c t="s" r="B69">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C69">
         <v>23820</v>
       </c>
+      <c t="n" r="D69">
+        <v>1</v>
+      </c>
+      <c t="s" r="E69">
+        <v>4</v>
+      </c>
       <c t="n" r="F69">
         <v>11</v>
       </c>
@@ -4410,25 +4602,31 @@
         <v>909</v>
       </c>
       <c t="s" r="J69">
-        <v>476</v>
+        <v>508</v>
       </c>
       <c t="s" r="K69">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c t="s" r="L69">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row spans="1:12" r="70">
       <c t="s" r="A70">
-        <v>258</v>
+        <v>282</v>
       </c>
       <c t="s" r="B70">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C70">
         <v>23933</v>
       </c>
+      <c t="n" r="D70">
+        <v>6</v>
+      </c>
+      <c t="s" r="E70">
+        <v>252</v>
+      </c>
       <c t="n" r="F70">
         <v>449</v>
       </c>
@@ -4442,25 +4640,31 @@
         <v>2277</v>
       </c>
       <c t="s" r="J70">
-        <v>424</v>
+        <v>456</v>
       </c>
       <c t="s" r="K70">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c t="s" r="L70">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row spans="1:12" r="71">
       <c t="s" r="A71">
-        <v>419</v>
+        <v>451</v>
       </c>
       <c t="s" r="B71">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C71">
         <v>23692</v>
       </c>
+      <c t="n" r="D71">
+        <v>4</v>
+      </c>
+      <c t="s" r="E71">
+        <v>271</v>
+      </c>
       <c t="n" r="F71">
         <v>29</v>
       </c>
@@ -4474,25 +4678,31 @@
         <v>939</v>
       </c>
       <c t="s" r="J71">
-        <v>353</v>
+        <v>385</v>
       </c>
       <c t="s" r="K71">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c t="s" r="L71">
-        <v>74</v>
+        <v>76</v>
       </c>
     </row>
     <row spans="1:12" r="72">
       <c t="s" r="A72">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c t="s" r="B72">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C72">
         <v>23682</v>
       </c>
+      <c t="n" r="D72">
+        <v>4</v>
+      </c>
+      <c t="s" r="E72">
+        <v>254</v>
+      </c>
       <c t="n" r="F72">
         <v>55</v>
       </c>
@@ -4506,25 +4716,31 @@
         <v>1032</v>
       </c>
       <c t="s" r="J72">
-        <v>430</v>
+        <v>462</v>
       </c>
       <c t="s" r="K72">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c t="s" r="L72">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row spans="1:12" r="73">
       <c t="s" r="A73">
-        <v>379</v>
+        <v>411</v>
       </c>
       <c t="s" r="B73">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C73">
         <v>23900</v>
       </c>
+      <c t="n" r="D73">
+        <v>6</v>
+      </c>
+      <c t="s" r="E73">
+        <v>179</v>
+      </c>
       <c t="n" r="F73">
         <v>570</v>
       </c>
@@ -4538,25 +4754,31 @@
         <v>2592</v>
       </c>
       <c t="s" r="J73">
-        <v>443</v>
+        <v>475</v>
       </c>
       <c t="s" r="K73">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c t="s" r="L73">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row spans="1:12" r="74">
       <c t="s" r="A74">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c t="s" r="B74">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C74">
         <v>23754</v>
       </c>
+      <c t="n" r="D74">
+        <v>5</v>
+      </c>
+      <c t="s" r="E74">
+        <v>180</v>
+      </c>
       <c t="n" r="F74">
         <v>163</v>
       </c>
@@ -4570,25 +4792,31 @@
         <v>1434</v>
       </c>
       <c t="s" r="J74">
-        <v>248</v>
+        <v>268</v>
       </c>
       <c t="s" r="K74">
-        <v>270</v>
+        <v>296</v>
       </c>
       <c t="s" r="L74">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row spans="1:12" r="75">
       <c t="s" r="A75">
-        <v>350</v>
+        <v>382</v>
       </c>
       <c t="s" r="B75">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C75">
         <v>23814</v>
       </c>
+      <c t="n" r="D75">
+        <v>5</v>
+      </c>
+      <c t="s" r="E75">
+        <v>333</v>
+      </c>
       <c t="n" r="F75">
         <v>11</v>
       </c>
@@ -4602,25 +4830,31 @@
         <v>927</v>
       </c>
       <c t="s" r="J75">
-        <v>475</v>
+        <v>507</v>
       </c>
       <c t="s" r="K75">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c t="s" r="L75">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row spans="1:12" r="76">
       <c t="s" r="A76">
-        <v>461</v>
+        <v>493</v>
       </c>
       <c t="s" r="B76">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C76">
         <v>23595</v>
       </c>
+      <c t="n" r="D76">
+        <v>3</v>
+      </c>
+      <c t="s" r="E76">
+        <v>250</v>
+      </c>
       <c t="n" r="F76">
         <v>19</v>
       </c>
@@ -4634,25 +4868,31 @@
         <v>867</v>
       </c>
       <c t="s" r="J76">
-        <v>222</v>
+        <v>235</v>
       </c>
       <c t="s" r="K76">
-        <v>266</v>
+        <v>292</v>
       </c>
       <c t="s" r="L76">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row spans="1:12" r="77">
       <c t="s" r="A77">
-        <v>408</v>
+        <v>440</v>
       </c>
       <c t="s" r="B77">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C77">
         <v>23395</v>
       </c>
+      <c t="n" r="D77">
+        <v>1</v>
+      </c>
+      <c t="s" r="E77">
+        <v>224</v>
+      </c>
       <c t="n" r="F77">
         <v>1</v>
       </c>
@@ -4666,25 +4906,31 @@
         <v>906</v>
       </c>
       <c t="s" r="J77">
-        <v>369</v>
+        <v>401</v>
       </c>
       <c t="s" r="K77">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c t="s" r="L77">
-        <v>97</v>
+        <v>99</v>
       </c>
     </row>
     <row spans="1:12" r="78">
       <c t="s" r="A78">
-        <v>462</v>
+        <v>494</v>
       </c>
       <c t="s" r="B78">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C78">
         <v>23818</v>
       </c>
+      <c t="n" r="D78">
+        <v>5</v>
+      </c>
+      <c t="s" r="E78">
+        <v>334</v>
+      </c>
       <c t="n" r="F78">
         <v>16</v>
       </c>
@@ -4698,25 +4944,31 @@
         <v>939</v>
       </c>
       <c t="s" r="J78">
-        <v>240</v>
+        <v>260</v>
       </c>
       <c t="s" r="K78">
-        <v>264</v>
+        <v>290</v>
       </c>
       <c t="s" r="L78">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row spans="1:12" r="79">
       <c t="s" r="A79">
-        <v>347</v>
+        <v>379</v>
       </c>
       <c t="s" r="B79">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C79">
         <v>23813</v>
       </c>
+      <c t="n" r="D79">
+        <v>5</v>
+      </c>
+      <c t="s" r="E79">
+        <v>332</v>
+      </c>
       <c t="n" r="F79">
         <v>15</v>
       </c>
@@ -4730,25 +4982,31 @@
         <v>948</v>
       </c>
       <c t="s" r="J79">
-        <v>435</v>
+        <v>467</v>
       </c>
       <c t="s" r="K79">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c t="s" r="L79">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row spans="1:12" r="80">
       <c t="s" r="A80">
-        <v>380</v>
+        <v>412</v>
       </c>
       <c t="s" r="B80">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C80">
         <v>23889</v>
       </c>
+      <c t="n" r="D80">
+        <v>6</v>
+      </c>
+      <c t="s" r="E80">
+        <v>166</v>
+      </c>
       <c t="n" r="F80">
         <v>1056</v>
       </c>
@@ -4762,25 +5020,31 @@
         <v>4092</v>
       </c>
       <c t="s" r="J80">
-        <v>282</v>
+        <v>308</v>
       </c>
       <c t="s" r="K80">
-        <v>289</v>
+        <v>315</v>
       </c>
       <c t="s" r="L80">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row spans="1:12" r="81">
       <c t="s" r="A81">
-        <v>411</v>
+        <v>443</v>
       </c>
       <c t="s" r="B81">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C81">
         <v>23713</v>
       </c>
+      <c t="n" r="D81">
+        <v>4</v>
+      </c>
+      <c t="s" r="E81">
+        <v>287</v>
+      </c>
       <c t="n" r="F81">
         <v>291</v>
       </c>
@@ -4794,25 +5058,31 @@
         <v>1773</v>
       </c>
       <c t="s" r="J81">
-        <v>451</v>
+        <v>483</v>
       </c>
       <c t="s" r="K81">
-        <v>469</v>
+        <v>501</v>
       </c>
       <c t="s" r="L81">
-        <v>152</v>
+        <v>154</v>
       </c>
     </row>
     <row spans="1:12" r="82">
       <c t="s" r="A82">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c t="s" r="B82">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C82">
         <v>23678</v>
       </c>
+      <c t="n" r="D82">
+        <v>4</v>
+      </c>
+      <c t="s" r="E82">
+        <v>225</v>
+      </c>
       <c t="n" r="F82">
         <v>1</v>
       </c>
@@ -4826,25 +5096,31 @@
         <v>1005</v>
       </c>
       <c t="s" r="J82">
-        <v>399</v>
+        <v>431</v>
       </c>
       <c t="s" r="K82">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c t="s" r="L82">
-        <v>140</v>
+        <v>142</v>
       </c>
     </row>
     <row spans="1:12" r="83">
       <c t="s" r="A83">
-        <v>421</v>
+        <v>453</v>
       </c>
       <c t="s" r="B83">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C83">
         <v>23691</v>
       </c>
+      <c t="n" r="D83">
+        <v>4</v>
+      </c>
+      <c t="s" r="E83">
+        <v>252</v>
+      </c>
       <c t="n" r="F83">
         <v>57</v>
       </c>
@@ -4858,25 +5134,31 @@
         <v>1080</v>
       </c>
       <c t="s" r="J83">
-        <v>304</v>
+        <v>336</v>
       </c>
       <c t="s" r="K83">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c t="s" r="L83">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row spans="1:12" r="84">
       <c t="s" r="A84">
-        <v>391</v>
+        <v>423</v>
       </c>
       <c t="s" r="B84">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C84">
         <v>23555</v>
       </c>
+      <c t="n" r="D84">
+        <v>3</v>
+      </c>
+      <c t="s" r="E84">
+        <v>167</v>
+      </c>
       <c t="n" r="F84">
         <v>55</v>
       </c>
@@ -4890,25 +5172,31 @@
         <v>1200</v>
       </c>
       <c t="s" r="J84">
-        <v>239</v>
+        <v>259</v>
       </c>
       <c t="s" r="K84">
-        <v>265</v>
+        <v>291</v>
       </c>
       <c t="s" r="L84">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row spans="1:12" r="85">
       <c t="s" r="A85">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c t="s" r="B85">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C85">
         <v>23843</v>
       </c>
+      <c t="n" r="D85">
+        <v>2</v>
+      </c>
+      <c t="s" r="E85">
+        <v>251</v>
+      </c>
       <c t="n" r="F85">
         <v>210</v>
       </c>
@@ -4922,25 +5210,31 @@
         <v>1593</v>
       </c>
       <c t="s" r="J85">
-        <v>466</v>
+        <v>498</v>
       </c>
       <c t="s" r="K85">
-        <v>470</v>
+        <v>502</v>
       </c>
       <c t="s" r="L85">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row spans="1:12" r="86">
       <c t="s" r="A86">
-        <v>365</v>
+        <v>397</v>
       </c>
       <c t="s" r="B86">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C86">
         <v>23426</v>
       </c>
+      <c t="n" r="D86">
+        <v>1</v>
+      </c>
+      <c t="s" r="E86">
+        <v>288</v>
+      </c>
       <c t="n" r="F86">
         <v>24</v>
       </c>
@@ -4954,25 +5248,31 @@
         <v>1041</v>
       </c>
       <c t="s" r="J86">
-        <v>431</v>
+        <v>463</v>
       </c>
       <c t="s" r="K86">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c t="s" r="L86">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row spans="1:12" r="87">
       <c t="s" r="A87">
-        <v>413</v>
+        <v>445</v>
       </c>
       <c t="s" r="B87">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C87">
         <v>23833</v>
       </c>
+      <c t="n" r="D87">
+        <v>1</v>
+      </c>
+      <c t="s" r="E87">
+        <v>257</v>
+      </c>
       <c t="n" r="F87">
         <v>383</v>
       </c>
@@ -4986,25 +5286,31 @@
         <v>2043</v>
       </c>
       <c t="s" r="J87">
-        <v>299</v>
+        <v>325</v>
       </c>
       <c t="s" r="K87">
-        <v>291</v>
+        <v>317</v>
       </c>
       <c t="s" r="L87">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row spans="1:12" r="88">
       <c t="s" r="A88">
-        <v>366</v>
+        <v>398</v>
       </c>
       <c t="s" r="B88">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C88">
         <v>23790</v>
       </c>
+      <c t="n" r="D88">
+        <v>5</v>
+      </c>
+      <c t="s" r="E88">
+        <v>274</v>
+      </c>
       <c t="n" r="F88">
         <v>33</v>
       </c>
@@ -5018,25 +5324,31 @@
         <v>1047</v>
       </c>
       <c t="s" r="J88">
-        <v>246</v>
+        <v>266</v>
       </c>
       <c t="s" r="K88">
-        <v>271</v>
+        <v>297</v>
       </c>
       <c t="s" r="L88">
-        <v>98</v>
+        <v>100</v>
       </c>
     </row>
     <row spans="1:12" r="89">
       <c t="s" r="A89">
-        <v>368</v>
+        <v>400</v>
       </c>
       <c t="s" r="B89">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C89">
         <v>23716</v>
       </c>
+      <c t="n" r="D89">
+        <v>4</v>
+      </c>
+      <c t="s" r="E89">
+        <v>329</v>
+      </c>
       <c t="n" r="F89">
         <v>48</v>
       </c>
@@ -5050,25 +5362,31 @@
         <v>1110</v>
       </c>
       <c t="s" r="J89">
-        <v>219</v>
+        <v>232</v>
       </c>
       <c t="s" r="K89">
-        <v>276</v>
+        <v>302</v>
       </c>
       <c t="s" r="L89">
-        <v>138</v>
+        <v>140</v>
       </c>
     </row>
     <row spans="1:12" r="90">
       <c t="s" r="A90">
-        <v>387</v>
+        <v>419</v>
       </c>
       <c t="s" r="B90">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C90">
         <v>23865</v>
       </c>
+      <c t="n" r="D90">
+        <v>5</v>
+      </c>
+      <c t="s" r="E90">
+        <v>330</v>
+      </c>
       <c t="n" r="F90">
         <v>1</v>
       </c>
@@ -5082,25 +5400,31 @@
         <v>1080</v>
       </c>
       <c t="s" r="J90">
-        <v>401</v>
+        <v>433</v>
       </c>
       <c t="s" r="K90">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c t="s" r="L90">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row spans="1:12" r="91">
       <c t="s" r="A91">
-        <v>488</v>
+        <v>520</v>
       </c>
       <c t="s" r="B91">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C91">
         <v>23496</v>
       </c>
+      <c t="n" r="D91">
+        <v>2</v>
+      </c>
+      <c t="s" r="E91">
+        <v>256</v>
+      </c>
       <c t="n" r="F91">
         <v>3</v>
       </c>
@@ -5114,25 +5438,31 @@
         <v>1092</v>
       </c>
       <c t="s" r="J91">
-        <v>442</v>
+        <v>474</v>
       </c>
       <c t="s" r="K91">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c t="s" r="L91">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row spans="1:12" r="92">
       <c t="s" r="A92">
-        <v>386</v>
+        <v>418</v>
       </c>
       <c t="s" r="B92">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C92">
         <v>23739</v>
       </c>
+      <c t="n" r="D92">
+        <v>5</v>
+      </c>
+      <c t="s" r="E92">
+        <v>165</v>
+      </c>
       <c t="n" r="F92">
         <v>1</v>
       </c>
@@ -5146,25 +5476,31 @@
         <v>1056</v>
       </c>
       <c t="s" r="J92">
-        <v>400</v>
+        <v>432</v>
       </c>
       <c t="s" r="K92">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c t="s" r="L92">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row spans="1:12" r="93">
       <c t="s" r="A93">
-        <v>383</v>
+        <v>415</v>
       </c>
       <c t="s" r="B93">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C93">
         <v>23509</v>
       </c>
+      <c t="n" r="D93">
+        <v>2</v>
+      </c>
+      <c t="s" r="E93">
+        <v>275</v>
+      </c>
       <c t="n" r="F93">
         <v>1</v>
       </c>
@@ -5178,25 +5514,31 @@
         <v>1137</v>
       </c>
       <c t="s" r="J93">
-        <v>361</v>
+        <v>393</v>
       </c>
       <c t="s" r="K93">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c t="s" r="L93">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row spans="1:12" r="94">
       <c t="s" r="A94">
-        <v>241</v>
+        <v>261</v>
       </c>
       <c t="s" r="B94">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C94">
         <v>23911</v>
       </c>
+      <c t="n" r="D94">
+        <v>6</v>
+      </c>
+      <c t="s" r="E94">
+        <v>227</v>
+      </c>
       <c t="n" r="F94">
         <v>606</v>
       </c>
@@ -5210,25 +5552,31 @@
         <v>2841</v>
       </c>
       <c t="s" r="J94">
-        <v>479</v>
+        <v>511</v>
       </c>
       <c t="s" r="K94">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c t="s" r="L94">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row spans="1:12" r="95">
       <c t="s" r="A95">
-        <v>341</v>
+        <v>373</v>
       </c>
       <c t="s" r="B95">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C95">
         <v>23495</v>
       </c>
+      <c t="n" r="D95">
+        <v>2</v>
+      </c>
+      <c t="s" r="E95">
+        <v>255</v>
+      </c>
       <c t="n" r="F95">
         <v>2</v>
       </c>
@@ -5242,25 +5590,31 @@
         <v>1053</v>
       </c>
       <c t="s" r="J95">
-        <v>292</v>
+        <v>318</v>
       </c>
       <c t="s" r="K95">
-        <v>287</v>
+        <v>313</v>
       </c>
       <c t="s" r="L95">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row spans="1:12" r="96">
       <c t="s" r="A96">
-        <v>255</v>
+        <v>279</v>
       </c>
       <c t="s" r="B96">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C96">
         <v>23876</v>
       </c>
+      <c t="n" r="D96">
+        <v>6</v>
+      </c>
+      <c t="s" r="E96">
+        <v>7</v>
+      </c>
       <c t="n" r="F96">
         <v>448</v>
       </c>
@@ -5274,25 +5628,31 @@
         <v>2466</v>
       </c>
       <c t="s" r="J96">
-        <v>340</v>
+        <v>372</v>
       </c>
       <c t="s" r="K96">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c t="s" r="L96">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row spans="1:12" r="97">
       <c t="s" r="A97">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c t="s" r="B97">
-        <v>496</v>
+        <v>528</v>
       </c>
       <c t="n" r="C97">
         <v>23871</v>
       </c>
+      <c t="n" r="D97">
+        <v>6</v>
+      </c>
+      <c t="s" r="E97">
+        <v>288</v>
+      </c>
       <c t="n" r="F97">
         <v>4</v>
       </c>
@@ -5306,13 +5666,13 @@
         <v>1416</v>
       </c>
       <c t="s" r="J97">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c t="s" r="K97">
-        <v>279</v>
+        <v>305</v>
       </c>
       <c t="s" r="L97">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>